<commit_message>
dedicate only one column for a dependee in dependency section.
</commit_message>
<xml_diff>
--- a/inheritance_and_dependencies/dependency_2.xlsx
+++ b/inheritance_and_dependencies/dependency_2.xlsx
@@ -380,7 +380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -392,13 +392,12 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="n"/>
       <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Parent</t>
+        </is>
+      </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Parent</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Methods/Children</t>
         </is>
@@ -410,12 +409,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>CarPollutionPermit</t>
         </is>
@@ -423,8 +417,7 @@
     </row>
     <row r="3">
       <c r="C3" s="2" t="n"/>
-      <c r="D3" s="2" t="n"/>
-      <c r="F3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -432,8 +425,7 @@
     </row>
     <row r="4">
       <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-      <c r="F4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
@@ -446,8 +438,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n"/>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>BikePollutionPermit</t>
         </is>
@@ -456,8 +447,7 @@
     <row r="6">
       <c r="B6" s="2" t="n"/>
       <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
-      <c r="F6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -466,8 +456,7 @@
     <row r="7">
       <c r="B7" s="2" t="n"/>
       <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n"/>
-      <c r="F7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
@@ -476,8 +465,7 @@
     <row r="8">
       <c r="B8" s="2" t="n"/>
       <c r="C8" s="2" t="n"/>
-      <c r="D8" s="2" t="n"/>
-      <c r="E8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>TractorPollutionPermit</t>
         </is>
@@ -486,8 +474,7 @@
     <row r="9">
       <c r="B9" s="2" t="n"/>
       <c r="C9" s="2" t="n"/>
-      <c r="D9" s="2" t="n"/>
-      <c r="F9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>fetch_tractor</t>
         </is>
@@ -496,8 +483,7 @@
     <row r="10">
       <c r="B10" s="2" t="n"/>
       <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n"/>
-      <c r="F10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
         </is>
@@ -506,8 +492,7 @@
     <row r="11">
       <c r="B11" s="2" t="n"/>
       <c r="C11" s="2" t="n"/>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
         </is>
@@ -516,8 +501,7 @@
     <row r="12">
       <c r="B12" s="2" t="n"/>
       <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="n"/>
-      <c r="F12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
         </is>
@@ -526,8 +510,7 @@
     <row r="13">
       <c r="B13" s="2" t="n"/>
       <c r="C13" s="2" t="n"/>
-      <c r="D13" s="2" t="n"/>
-      <c r="E13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Vehicle</t>
         </is>
@@ -536,8 +519,7 @@
     <row r="14">
       <c r="B14" s="2" t="n"/>
       <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
-      <c r="F14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -546,8 +528,7 @@
     <row r="15">
       <c r="B15" s="2" t="n"/>
       <c r="C15" s="2" t="n"/>
-      <c r="D15" s="2" t="n"/>
-      <c r="F15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>mileage_calculator</t>
         </is>
@@ -556,8 +537,7 @@
     <row r="16">
       <c r="B16" s="2" t="n"/>
       <c r="C16" s="2" t="n"/>
-      <c r="D16" s="2" t="n"/>
-      <c r="F16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Car</t>
         </is>
@@ -566,8 +546,7 @@
     <row r="17">
       <c r="B17" s="2" t="n"/>
       <c r="C17" s="2" t="n"/>
-      <c r="D17" s="2" t="n"/>
-      <c r="F17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Bike</t>
         </is>
@@ -575,13 +554,12 @@
     </row>
     <row r="18">
       <c r="B18" s="2" t="n"/>
-      <c r="C18" s="2" t="n"/>
-      <c r="D18" s="2" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Car</t>
         </is>
@@ -590,7 +568,7 @@
     <row r="19">
       <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="n"/>
-      <c r="F19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -599,7 +577,7 @@
     <row r="20">
       <c r="B20" s="2" t="n"/>
       <c r="C20" s="2" t="n"/>
-      <c r="F20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>pollution_permit</t>
         </is>
@@ -613,7 +591,7 @@
       </c>
       <c r="B21" s="2" t="n"/>
       <c r="C21" s="2" t="n"/>
-      <c r="E21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Farzi</t>
         </is>
@@ -623,7 +601,7 @@
       <c r="A22" s="2" t="n"/>
       <c r="B22" s="2" t="n"/>
       <c r="C22" s="2" t="n"/>
-      <c r="F22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -633,7 +611,7 @@
       <c r="A23" s="2" t="n"/>
       <c r="B23" s="2" t="n"/>
       <c r="C23" s="2" t="n"/>
-      <c r="F23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>
@@ -655,28 +633,28 @@
           <t>←</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Bike</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="F25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="F26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>pollution_permit</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="F27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>

</xml_diff>

<commit_message>
completes indentation and navigation
</commit_message>
<xml_diff>
--- a/inheritance_and_dependencies/dependency_2.xlsx
+++ b/inheritance_and_dependencies/dependency_2.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="class_to_child_and_dependents" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="sheet_one" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -387,6 +387,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="4" min="4" width="8.4"/>
+    <col customWidth="1" max="5" min="5" width="22.8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
@@ -661,6 +665,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E16" r:id="rId2"/>
+    <hyperlink ref="E17" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>